<commit_message>
Assign biomass to 100% guaranteed dispatch
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\India\Models\eps-india\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BGDPbES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -591,99 +591,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="58.28515625" customWidth="1"/>
+    <col min="1" max="1" width="58.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>2010</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -702,17 +702,17 @@
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.59765625" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -825,7 +825,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -973,7 +973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1861,155 +1861,155 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
         <f t="shared" ref="D9:AK17" si="2">$B9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK9">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>0.106</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Edit to About page text for BGDPbES
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Notes:</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Sec 6.5 (11). Pp 176 - must-run for all RE except Biomass and Cogen</t>
   </si>
   <si>
-    <t xml:space="preserve">For India, we dispatch 100% to wind, solar and as per must-run status </t>
-  </si>
-  <si>
     <t>accorded to these sources in IEGC.</t>
   </si>
   <si>
@@ -130,6 +127,12 @@
   </si>
   <si>
     <t>municipal solid waste</t>
+  </si>
+  <si>
+    <t>Biomass source is also guaranteed to ensure it is dispatched based on price in the model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For India, we dispatch 100% to wind and solar as per must-run status </t>
   </si>
 </sst>
 </file>
@@ -589,9 +592,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -670,22 +675,27 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -714,7 +724,7 @@
   <sheetData>
     <row r="1" spans="1:37" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2">
         <v>2015</v>
@@ -2751,7 +2761,7 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2899,7 +2909,7 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -3047,7 +3057,7 @@
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>0</v>

</xml_diff>